<commit_message>
add more results to compare
</commit_message>
<xml_diff>
--- a/result_compare.xlsx
+++ b/result_compare.xlsx
@@ -15,12 +15,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="61">
   <si>
     <t>textrank method -1</t>
   </si>
   <si>
     <t>final result ==&gt; precision : 0.102685   recall : 0.287747   f : 0.146631</t>
+  </si>
+  <si>
+    <t>textrank method 0</t>
   </si>
   <si>
     <t>final result ==&gt; precision : 0.118647   recall : 0.332091   f : 0.169599</t>
@@ -37,9 +40,6 @@
 			S += 0.1</t>
   </si>
   <si>
-    <t>textrank method 0</t>
-  </si>
-  <si>
     <t>final result ==&gt; precision : 0.119330   recall : 0.333881   f : 0.170574</t>
   </si>
   <si>
@@ -54,8 +54,18 @@
 			S += 0.05</t>
   </si>
   <si>
-    <t>final result ==&gt; precision : 0.119391 	 recall : 0.334124 	 f : 0.170670
-</t>
+    <t>WEIGHT_LOC_RAND = 1.0
+WEIGHT_POS_RAND = 0.0
+s=0.0
+		if title:
+			s += 0.7
+		if first_sentences:
+			S += 0.2
+		if last_sentences:
+			S += 0.1</t>
+  </si>
+  <si>
+    <t>final result ==&gt; precision : 0.119391 	 recall : 0.334124 	 f : 0.170670</t>
   </si>
   <si>
     <t>WEIGHT_LOC_RAND = 1.0
@@ -112,6 +122,81 @@
 LAMBDA_LAST = 15</t>
   </si>
   <si>
+    <t>final result ==&gt; precision : 0.108069   recall : 0.302701   f : 0.154400</t>
+  </si>
+  <si>
+    <t>WEIGHT_COV = 0.1
+WEIGHT_LOC = 0.7
+WEIGHT_POS = 0.1
+WEIGHT_FREQ = 0.1
+LAMBDA_TITLE = 40
+LAMBDA_FIRST = 10
+LAMBDA_LAST = 10</t>
+  </si>
+  <si>
+    <t>final result ==&gt; precision : 0.108087   recall : 0.302710   f : 0.154421</t>
+  </si>
+  <si>
+    <t>WEIGHT_COV = 0.1
+WEIGHT_LOC = 0.7
+WEIGHT_POS = 0.1
+WEIGHT_FREQ = 0.1
+LAMBDA_TITLE = 50
+LAMBDA_FIRST = 10
+LAMBDA_LAST = 10</t>
+  </si>
+  <si>
+    <t>final result ==&gt; precision : 0.108268   recall : 0.303132   f : 0.154669</t>
+  </si>
+  <si>
+    <t>WEIGHT_COV = 0.1
+WEIGHT_LOC = 0.7
+WEIGHT_POS = 0.1
+WEIGHT_FREQ = 0.1
+LAMBDA_TITLE = 60
+LAMBDA_FIRST = 10
+LAMBDA_LAST = 10</t>
+  </si>
+  <si>
+    <t>final result ==&gt; precision : 0.108104   recall : 0.302722   f : 0.154430</t>
+  </si>
+  <si>
+    <t>WEIGHT_COV = 0.1
+WEIGHT_LOC = 0.7
+WEIGHT_POS = 0.1
+WEIGHT_FREQ = 0.1
+LAMBDA_TITLE = 80
+LAMBDA_FIRST = 10
+LAMBDA_LAST = 10</t>
+  </si>
+  <si>
+    <t>final result ==&gt; precision : 0.107490   recall : 0.301193   f : 0.153581</t>
+  </si>
+  <si>
+    <t>WEIGHT_COV = 0.1
+WEIGHT_LOC = 0.8
+WEIGHT_POS = 0.1
+WEIGHT_FREQ = 0.0
+LAMBDA_TITLE = 60
+LAMBDA_FIRST = 10
+LAMBDA_LAST = 10</t>
+  </si>
+  <si>
+    <t>final result ==&gt; precision : 0.107309   recall : 0.300477   f : 0.153296</t>
+  </si>
+  <si>
+    <t>WEIGHT_COV = 0.1
+WEIGHT_LOC = 0.8
+WEIGHT_POS = 0.1
+WEIGHT_FREQ = 0.0
+LAMBDA_TITLE = 80
+LAMBDA_FIRST = 10
+LAMBDA_LAST = 10</t>
+  </si>
+  <si>
+    <t>右</t>
+  </si>
+  <si>
     <t>final result ==&gt; precision : 0.107412   recall : 0.300999   f : 0.153474</t>
   </si>
   <si>
@@ -120,6 +205,635 @@
 WEIGHT_POS = 0.1
 WEIGHT_FREQ = 0.0
 LAMBDA_TITLE = 40
+LAMBDA_FIRST = 10
+LAMBDA_LAST = 10</t>
+  </si>
+  <si>
+    <t>final result ==&gt; precision : 0.107153   recall : 0.300384   f : 0.153108</t>
+  </si>
+  <si>
+    <t>WEIGHT_COV = 0.2
+WEIGHT_LOC = 0.8
+WEIGHT_POS = 0.0
+WEIGHT_FREQ = 0.0
+LAMBDA_TITLE = 30
+LAMBDA_FIRST = 10
+LAMBDA_LAST = 10</t>
+  </si>
+  <si>
+    <t>final result ==&gt; precision : 0.107525   recall : 0.301167   f : 0.153620</t>
+  </si>
+  <si>
+    <t>WEIGHT_COV = 0.2
+WEIGHT_LOC = 0.8
+WEIGHT_POS = 0.0
+WEIGHT_FREQ = 0.0
+LAMBDA_TITLE = 60
+LAMBDA_FIRST = 10
+LAMBDA_LAST = 10</t>
+  </si>
+  <si>
+    <t>下</t>
+  </si>
+  <si>
+    <t>final result ==&gt; precision : 0.106704   recall : 0.298980   f : 0.152442</t>
+  </si>
+  <si>
+    <t>WEIGHT_COV = 0.0
+WEIGHT_LOC = 0.9
+WEIGHT_POS = 0.1
+WEIGHT_FREQ = 0.0
+LAMBDA_TITLE = 80
+LAMBDA_FIRST = 10
+LAMBDA_LAST = 10</t>
+  </si>
+  <si>
+    <t>final result ==&gt; precision : 0.109072   recall : 0.305331   f : 0.155827</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">WEIGHT_COV = 0.1
+WEIGHT_LOC = 0.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">６
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">WEIGHT_POS = 0.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">２
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">WEIGHT_FREQ = 0.1
+LAMBDA_TITLE = 60
+LAMBDA_FIRST = 10
+LAMBDA_LAST = 10</t>
+    </r>
+  </si>
+  <si>
+    <t>final result ==&gt; precision : 0.109054   recall : 0.305250   f : 0.155797</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">WEIGHT_COV = 0.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">２
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">WEIGHT_LOC = 0.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">６
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">WEIGHT_POS = 0.1
+WEIGHT_FREQ = 0.1
+LAMBDA_TITLE = 60
+LAMBDA_FIRST = 10
+LAMBDA_LAST = 10</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">WEIGHT_COV = 0.1
+WEIGHT_LOC = 0.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">６
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">WEIGHT_POS = 0.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">１
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">WEIGHT_FREQ = 0.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">２
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">LAMBDA_TITLE = 60
+LAMBDA_FIRST = 10
+LAMBDA_LAST = 10</t>
+    </r>
+  </si>
+  <si>
+    <t>final result ==&gt; precision : 0.111068   recall : 0.310472   f : 0.158657</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">WEIGHT_COV = 0.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">３
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">WEIGHT_LOC = 0.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">３
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">WEIGHT_POS = 0.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">２
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">WEIGHT_FREQ = 0.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">２
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">LAMBDA_TITLE = 60
+LAMBDA_FIRST = 10
+LAMBDA_LAST = 10</t>
+    </r>
+  </si>
+  <si>
+    <t>final result ==&gt; precision : 0.111068   recall : 0.310483   f : 0.158658</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">WEIGHT_COV = 0.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">２
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">WEIGHT_LOC = 0.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">３
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">WEIGHT_POS = 0.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">３
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">WEIGHT_FREQ = 0.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">２
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">LAMBDA_TITLE = 60
+LAMBDA_FIRST = 10
+LAMBDA_LAST = 10</t>
+    </r>
+  </si>
+  <si>
+    <t>final result ==&gt; precision : 0.110420   recall : 0.308219   f : 0.157684</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">WEIGHT_COV = 0.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">２
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">WEIGHT_LOC = 0.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">２
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">WEIGHT_POS = 0.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">３
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">WEIGHT_FREQ = 0.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">３
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">LAMBDA_TITLE = 60
+LAMBDA_FIRST = 10
+LAMBDA_LAST = 10</t>
+    </r>
+  </si>
+  <si>
+    <t>final result ==&gt; precision : 0.110446   recall : 0.308320   f : 0.157723</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">WEIGHT_COV = 0.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">３
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">WEIGHT_LOC = 0.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">２
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">WEIGHT_POS = 0.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">２
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">WEIGHT_FREQ = 0.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">３
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">LAMBDA_TITLE = 60
+LAMBDA_FIRST = 10
+LAMBDA_LAST = 10</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">WEIGHT_COV = 0.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">３
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">WEIGHT_LOC = 0.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">３
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">WEIGHT_POS = 0.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">３
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">WEIGHT_FREQ = 0.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">１
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">LAMBDA_TITLE = 60
+LAMBDA_FIRST = 10
+LAMBDA_LAST = 10</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">textrank method </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">２</t>
+    </r>
+  </si>
+  <si>
+    <t>final result ==&gt; precision : 0.099755   recall : 0.279378   f : 0.142405</t>
+  </si>
+  <si>
+    <t>WEIGHT_COV = 0.0
+WEIGHT_LOC = 0.0
+WEIGHT_POS = 0.1
+WEIGHT_FREQ = 0.9
+LAMBDA_TITLE = 60
+LAMBDA_FIRST = 10
+LAMBDA_LAST = 10</t>
+  </si>
+  <si>
+    <t>you</t>
+  </si>
+  <si>
+    <t>final result ==&gt; precision : 0.107369   recall : 0.300247   f : 0.153321</t>
+  </si>
+  <si>
+    <t>WEIGHT_COV = 0.0
+WEIGHT_LOC = 0.1
+WEIGHT_POS = 0.1
+WEIGHT_FREQ = 0.8
+LAMBDA_TITLE = 60
+LAMBDA_FIRST = 10
+LAMBDA_LAST = 10</t>
+  </si>
+  <si>
+    <t>final result ==&gt; precision : 0.109080   recall : 0.305264   f : 0.155831</t>
+  </si>
+  <si>
+    <t>WEIGHT_COV = 0.4
+WEIGHT_LOC = 0.6
+WEIGHT_POS = 0.0
+WEIGHT_FREQ = 0.0
+LAMBDA_TITLE = 60
 LAMBDA_FIRST = 10
 LAMBDA_LAST = 10</t>
   </si>
@@ -131,11 +845,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <name val="Droid Sans Fallback"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -156,12 +871,38 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFFF3333"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Droid Sans Fallback"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF3333"/>
+      <name val="Droid Sans Fallback"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -206,12 +947,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -221,6 +966,26 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -300,10 +1065,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A29" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C35" activeCellId="0" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -311,7 +1076,8 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.6701030927835"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="64.2886597938144"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.6030927835052"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.639175257732"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.9639175257732"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.639175257732"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -325,66 +1091,268 @@
         <v>11571</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="122.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="B2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="C2" s="3" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="3" t="s">
+    <row r="4" customFormat="false" ht="102.2" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="2" t="s">
+    </row>
+    <row r="5" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="3" t="s">
         <v>9</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="2" t="s">
+    </row>
+    <row r="7" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
+      <c r="C7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="1" t="s">
+    </row>
+    <row r="8" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="1" t="s">
+      <c r="C8" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="2" t="s">
+    </row>
+    <row r="9" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1" t="s">
         <v>17</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="104.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1"/>
+      <c r="B11" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="104.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="84.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="88.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="88.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B23" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="88.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="88.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="88.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>